<commit_message>
valorizzare le seguenti colonne: M, N, P, Q, R, S
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IG.PSO/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IG.PSO/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IG.PSO\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDBF2A6-FFDD-49ED-88CE-7D1CB6519463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9869821A-DA6F-4070-B498-EB29CD758385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="577">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3066,6 +3066,9 @@
     <xf numFmtId="164" fontId="4" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3088,9 +3091,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4539,13 +4539,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T34" sqref="T34"/>
+      <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4587,14 +4588,14 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="59" t="s">
         <v>437</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="60"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4615,14 +4616,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="66" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="67" t="s">
         <v>438</v>
       </c>
-      <c r="D3" s="57"/>
+      <c r="D3" s="58"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4643,12 +4644,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="66" t="s">
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="67" t="s">
         <v>440</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4670,12 +4671,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="66" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="57"/>
+      <c r="D5" s="58"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4696,8 +4697,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -4832,7 +4833,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -4869,7 +4870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="35">
         <v>28</v>
       </c>
@@ -4906,7 +4907,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -4943,7 +4944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="35">
         <v>30</v>
       </c>
@@ -4980,7 +4981,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -5054,7 +5055,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="35">
         <v>33</v>
       </c>
@@ -5091,7 +5092,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="35">
         <v>34</v>
       </c>
@@ -5171,7 +5172,9 @@
       <c r="R18" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S18" s="45"/>
+      <c r="S18" s="45" t="s">
+        <v>449</v>
+      </c>
       <c r="T18" s="45" t="s">
         <v>226</v>
       </c>
@@ -5183,7 +5186,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="35">
         <v>36</v>
       </c>
@@ -5220,7 +5223,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -5257,7 +5260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="35">
         <v>38</v>
       </c>
@@ -5294,7 +5297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -5368,7 +5371,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="35">
         <v>41</v>
       </c>
@@ -5405,7 +5408,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="35">
         <v>42</v>
       </c>
@@ -5485,7 +5488,9 @@
       <c r="R26" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S26" s="45"/>
+      <c r="S26" s="45" t="s">
+        <v>449</v>
+      </c>
       <c r="T26" s="45" t="s">
         <v>226</v>
       </c>
@@ -5497,7 +5502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="35">
         <v>44</v>
       </c>
@@ -5536,7 +5541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="35">
         <v>45</v>
       </c>
@@ -5575,7 +5580,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="35">
         <v>46</v>
       </c>
@@ -5614,7 +5619,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -5653,7 +5658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="35">
         <v>48</v>
       </c>
@@ -5692,7 +5697,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="35">
         <v>49</v>
       </c>
@@ -5731,7 +5736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="35">
         <v>50</v>
       </c>
@@ -5815,7 +5820,9 @@
       <c r="R34" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S34" s="45"/>
+      <c r="S34" s="45" t="s">
+        <v>449</v>
+      </c>
       <c r="T34" s="45" t="s">
         <v>226</v>
       </c>
@@ -5829,7 +5836,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="35">
         <v>53</v>
       </c>
@@ -5866,7 +5873,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="35">
         <v>55</v>
       </c>
@@ -5903,7 +5910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="35">
         <v>56</v>
       </c>
@@ -5940,7 +5947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="35">
         <v>57</v>
       </c>
@@ -5977,7 +5984,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="35">
         <v>59</v>
       </c>
@@ -6014,7 +6021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="35">
         <v>60</v>
       </c>
@@ -6051,7 +6058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="35">
         <v>61</v>
       </c>
@@ -6088,7 +6095,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="35">
         <v>62</v>
       </c>
@@ -6125,7 +6132,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="35">
         <v>64</v>
       </c>
@@ -6162,7 +6169,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="35">
         <v>66</v>
       </c>
@@ -6199,7 +6206,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="35">
         <v>67</v>
       </c>
@@ -6236,7 +6243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="35">
         <v>68</v>
       </c>
@@ -6273,7 +6280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="35">
         <v>69</v>
       </c>
@@ -6310,7 +6317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="35">
         <v>70</v>
       </c>
@@ -6347,7 +6354,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="35">
         <v>71</v>
       </c>
@@ -6384,7 +6391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="35">
         <v>72</v>
       </c>
@@ -6421,7 +6428,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="35">
         <v>73</v>
       </c>
@@ -6458,7 +6465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="35">
         <v>74</v>
       </c>
@@ -6495,7 +6502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="35">
         <v>76</v>
       </c>
@@ -6532,7 +6539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="35">
         <v>78</v>
       </c>
@@ -6569,7 +6576,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="35">
         <v>79</v>
       </c>
@@ -6606,7 +6613,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="35">
         <v>80</v>
       </c>
@@ -6643,7 +6650,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="35">
         <v>81</v>
       </c>
@@ -6680,7 +6687,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="35">
         <v>83</v>
       </c>
@@ -6717,7 +6724,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="35">
         <v>84</v>
       </c>
@@ -6754,7 +6761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="35">
         <v>85</v>
       </c>
@@ -6791,7 +6798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="35">
         <v>86</v>
       </c>
@@ -6828,7 +6835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="35">
         <v>87</v>
       </c>
@@ -6865,7 +6872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="35">
         <v>88</v>
       </c>
@@ -6902,7 +6909,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="35">
         <v>89</v>
       </c>
@@ -6939,7 +6946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="35">
         <v>90</v>
       </c>
@@ -6976,7 +6983,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="35">
         <v>91</v>
       </c>
@@ -7013,7 +7020,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="35">
         <v>92</v>
       </c>
@@ -7050,7 +7057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="35">
         <v>93</v>
       </c>
@@ -7087,7 +7094,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="35">
         <v>95</v>
       </c>
@@ -7124,7 +7131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="35">
         <v>97</v>
       </c>
@@ -7161,7 +7168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="35">
         <v>98</v>
       </c>
@@ -7198,7 +7205,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="35">
         <v>99</v>
       </c>
@@ -7235,7 +7242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="35">
         <v>100</v>
       </c>
@@ -7272,7 +7279,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="35">
         <v>101</v>
       </c>
@@ -7309,7 +7316,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="35">
         <v>102</v>
       </c>
@@ -7346,7 +7353,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="35">
         <v>103</v>
       </c>
@@ -7383,7 +7390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="35">
         <v>104</v>
       </c>
@@ -7420,7 +7427,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="35">
         <v>105</v>
       </c>
@@ -7457,7 +7464,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="35">
         <v>106</v>
       </c>
@@ -7494,7 +7501,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="35">
         <v>108</v>
       </c>
@@ -7531,7 +7538,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="35">
         <v>110</v>
       </c>
@@ -7568,7 +7575,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="35">
         <v>111</v>
       </c>
@@ -7605,7 +7612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="35">
         <v>112</v>
       </c>
@@ -7642,7 +7649,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="35">
         <v>113</v>
       </c>
@@ -7679,7 +7686,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="35">
         <v>114</v>
       </c>
@@ -7716,7 +7723,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="35">
         <v>115</v>
       </c>
@@ -7753,7 +7760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="35">
         <v>116</v>
       </c>
@@ -7790,7 +7797,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="35">
         <v>117</v>
       </c>
@@ -7827,7 +7834,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="35">
         <v>118</v>
       </c>
@@ -7864,7 +7871,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="35">
         <v>119</v>
       </c>
@@ -7901,7 +7908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="35">
         <v>120</v>
       </c>
@@ -7938,7 +7945,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="35">
         <v>121</v>
       </c>
@@ -9422,7 +9429,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="35">
         <v>152</v>
       </c>
@@ -9459,7 +9466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="35">
         <v>154</v>
       </c>
@@ -9496,7 +9503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="35">
         <v>155</v>
       </c>
@@ -9533,7 +9540,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="35">
         <v>156</v>
       </c>
@@ -9570,7 +9577,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="35">
         <v>159</v>
       </c>
@@ -9607,7 +9614,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="35">
         <v>160</v>
       </c>
@@ -9644,7 +9651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="35">
         <v>161</v>
       </c>
@@ -9681,7 +9688,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="35">
         <v>162</v>
       </c>
@@ -9718,7 +9725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="35">
         <v>163</v>
       </c>
@@ -9755,7 +9762,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="35">
         <v>164</v>
       </c>
@@ -9792,7 +9799,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="35">
         <v>165</v>
       </c>
@@ -9829,7 +9836,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="35">
         <v>166</v>
       </c>
@@ -9866,7 +9873,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="35">
         <v>167</v>
       </c>
@@ -9903,7 +9910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="35">
         <v>168</v>
       </c>
@@ -9940,7 +9947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="35">
         <v>169</v>
       </c>
@@ -9977,7 +9984,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="35">
         <v>175</v>
       </c>
@@ -10014,7 +10021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="35">
         <v>177</v>
       </c>
@@ -10051,7 +10058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="35">
         <v>178</v>
       </c>
@@ -10088,7 +10095,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="35">
         <v>179</v>
       </c>
@@ -10125,7 +10132,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="35">
         <v>180</v>
       </c>
@@ -10162,7 +10169,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="35">
         <v>181</v>
       </c>
@@ -10199,7 +10206,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="35">
         <v>182</v>
       </c>
@@ -10236,7 +10243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="35">
         <v>183</v>
       </c>
@@ -10273,7 +10280,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="35">
         <v>184</v>
       </c>
@@ -10310,7 +10317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="35">
         <v>185</v>
       </c>
@@ -10347,7 +10354,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="35">
         <v>186</v>
       </c>
@@ -10384,7 +10391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="35">
         <v>187</v>
       </c>
@@ -10421,7 +10428,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="35">
         <v>188</v>
       </c>
@@ -10458,7 +10465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="35">
         <v>189</v>
       </c>
@@ -10495,7 +10502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="35">
         <v>190</v>
       </c>
@@ -10532,7 +10539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="35">
         <v>191</v>
       </c>
@@ -10569,7 +10576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="35">
         <v>376</v>
       </c>
@@ -10606,7 +10613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="35">
         <v>417</v>
       </c>
@@ -10643,7 +10650,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="35">
         <v>418</v>
       </c>
@@ -10680,7 +10687,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="35">
         <v>419</v>
       </c>
@@ -10717,7 +10724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="35">
         <v>423</v>
       </c>
@@ -10754,7 +10761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="35">
         <v>424</v>
       </c>
@@ -10791,7 +10798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="35">
         <v>425</v>
       </c>
@@ -10828,7 +10835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -10865,7 +10872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -10902,7 +10909,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -10939,7 +10946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -10976,7 +10983,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -11013,7 +11020,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -11050,7 +11057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -11087,7 +11094,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -11124,7 +11131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -11161,7 +11168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -11198,7 +11205,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="35">
         <v>444</v>
       </c>
@@ -11235,7 +11242,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="35">
         <v>445</v>
       </c>
@@ -11272,7 +11279,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="35">
         <v>448</v>
       </c>
@@ -11309,7 +11316,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="35">
         <v>449</v>
       </c>
@@ -11346,7 +11353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="35">
         <v>450</v>
       </c>
@@ -11383,7 +11390,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="35">
         <v>451</v>
       </c>
@@ -11420,7 +11427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="35">
         <v>452</v>
       </c>
@@ -11490,13 +11497,25 @@
       </c>
       <c r="K171" s="45"/>
       <c r="L171" s="45"/>
-      <c r="M171" s="45"/>
-      <c r="N171" s="45"/>
+      <c r="M171" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="N171" s="45" t="s">
+        <v>228</v>
+      </c>
       <c r="O171" s="45"/>
-      <c r="P171" s="45"/>
-      <c r="Q171" s="45"/>
-      <c r="R171" s="45"/>
-      <c r="S171" s="45"/>
+      <c r="P171" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q171" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="R171" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="S171" s="45" t="s">
+        <v>449</v>
+      </c>
       <c r="T171" s="45"/>
       <c r="U171" s="51"/>
       <c r="V171" s="52" t="s">
@@ -11539,13 +11558,25 @@
       </c>
       <c r="K172" s="45"/>
       <c r="L172" s="45"/>
-      <c r="M172" s="45"/>
-      <c r="N172" s="45"/>
+      <c r="M172" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="N172" s="45" t="s">
+        <v>228</v>
+      </c>
       <c r="O172" s="45"/>
-      <c r="P172" s="45"/>
-      <c r="Q172" s="45"/>
-      <c r="R172" s="45"/>
-      <c r="S172" s="45"/>
+      <c r="P172" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q172" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="R172" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="S172" s="45" t="s">
+        <v>449</v>
+      </c>
       <c r="T172" s="45"/>
       <c r="U172" s="51"/>
       <c r="V172" s="52" t="s">
@@ -11555,7 +11586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="35">
         <v>456</v>
       </c>
@@ -11592,7 +11623,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="35">
         <v>457</v>
       </c>
@@ -11629,7 +11660,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="35">
         <v>458</v>
       </c>
@@ -11666,7 +11697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="35">
         <v>459</v>
       </c>
@@ -11703,7 +11734,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="35">
         <v>460</v>
       </c>
@@ -11740,7 +11771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="35">
         <v>461</v>
       </c>
@@ -11777,7 +11808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="35">
         <v>462</v>
       </c>
@@ -11830,7 +11861,7 @@
       <c r="E180" s="48" t="s">
         <v>393</v>
       </c>
-      <c r="F180" s="67" t="s">
+      <c r="F180" s="54" t="s">
         <v>565</v>
       </c>
       <c r="G180" s="46" t="s">
@@ -11877,7 +11908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="35">
         <v>464</v>
       </c>
@@ -11914,7 +11945,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="35">
         <v>465</v>
       </c>
@@ -11951,7 +11982,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="35">
         <v>466</v>
       </c>
@@ -11988,7 +12019,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="35">
         <v>467</v>
       </c>
@@ -12025,7 +12056,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="35">
         <v>468</v>
       </c>
@@ -12062,7 +12093,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="35">
         <v>469</v>
       </c>
@@ -12099,7 +12130,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="35">
         <v>470</v>
       </c>
@@ -12136,7 +12167,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="35">
         <v>471</v>
       </c>
@@ -12173,7 +12204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="35">
         <v>472</v>
       </c>
@@ -12210,7 +12241,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="35">
         <v>473</v>
       </c>
@@ -12247,7 +12278,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="35">
         <v>474</v>
       </c>
@@ -12284,7 +12315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:23" ht="140.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A192" s="35">
         <v>475</v>
       </c>
@@ -16338,7 +16369,13 @@
     <row r="751" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="752" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="VPS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -16359,7 +16396,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10:J192 P10:R192 M10:N192</xm:sqref>
+          <xm:sqref>J10:J192 M10:N192 P10:R192</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -18622,15 +18659,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18892,27 +18926,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18937,9 +18965,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
corretti errori test 30 e 31
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IG.PSO/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IG.PSO/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IG.PSO\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16772522-53A2-46B3-B1B2-D7D29B99AADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF17550-9EB1-43F2-8520-C8CA062BC57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2387,12 +2387,12 @@
   <si>
     <t>{
   "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "data": "2025-10-28T11:48:56.1108504Z",
+  "data": "2025-10-29T15:21:13.3467269Z",
   "status": 200,
-  "traceID": "de469be647a5ce39640f756508ecd8de",
-  "spanID": "d31ada44c223ed99",
+  "traceID": "c70bbf4796d250d971830ad55c4d9cc8",
+  "spanID": "e542cb5108db0e4e",
   "warning": null,
-  "workflowInstanceId": "2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.26bf06c765^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
+  "workflowInstanceId": "2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.a13b5bddeb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
   "type": null,
   "title": null,
   "detail": null,
@@ -2400,26 +2400,26 @@
 }</t>
   </si>
   <si>
-    <t>2025-10-28T11:48:56</t>
-  </si>
-  <si>
-    <t>2025-10-28</t>
-  </si>
-  <si>
-    <t>de469be647a5ce39640f756508ecd8de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.26bf06c765^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-10-29T15:21:13</t>
+  </si>
+  <si>
+    <t>c70bbf4796d250d971830ad55c4d9cc8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.a13b5bddeb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-10-29</t>
   </si>
   <si>
     <t>{
   "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "data": "2025-10-28T11:56:19.5413583Z",
+  "data": "2025-10-29T15:23:25.8267847Z",
   "status": 200,
-  "traceID": "82088edf0b094cd5801e1140192ea2a9",
-  "spanID": "65c4e71600be3e53",
+  "traceID": "3c3e3dd1b2548d8d8112fc300ba4129e",
+  "spanID": "121284dc82c7d403",
   "warning": null,
-  "workflowInstanceId": "2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.20d6555be3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
+  "workflowInstanceId": "2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.d51b7f90a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
   "type": null,
   "title": null,
   "detail": null,
@@ -2427,13 +2427,13 @@
 }</t>
   </si>
   <si>
-    <t>2025-10-28T11:56:19</t>
-  </si>
-  <si>
-    <t>82088edf0b094cd5801e1140192ea2a9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.20d6555be3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-10-29T15:23:25</t>
+  </si>
+  <si>
+    <t>3c3e3dd1b2548d8d8112fc300ba4129e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.d51b7f90a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3072,6 +3072,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3095,7 +3096,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{565105C8-FFD6-432C-8B2E-BD1D172FCD26}"/>
@@ -4550,7 +4550,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="E115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A171" sqref="A171:XFD172"/>
+      <selection pane="bottomRight" activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4592,14 +4592,14 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60" t="s">
         <v>437</v>
       </c>
-      <c r="D2" s="60"/>
+      <c r="D2" s="61"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4620,14 +4620,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="67" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="68" t="s">
         <v>438</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="59"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4648,12 +4648,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="67" t="s">
+      <c r="A4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="68" t="s">
         <v>440</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4675,12 +4675,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="68" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4701,8 +4701,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -11468,7 +11468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" s="68" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" s="55" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="46">
         <v>454</v>
       </c>
@@ -11485,16 +11485,16 @@
         <v>381</v>
       </c>
       <c r="F171" s="53" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="G171" s="49" t="s">
         <v>570</v>
       </c>
       <c r="H171" s="49" t="s">
+        <v>571</v>
+      </c>
+      <c r="I171" s="50" t="s">
         <v>572</v>
-      </c>
-      <c r="I171" s="50" t="s">
-        <v>573</v>
       </c>
       <c r="J171" s="45" t="s">
         <v>64</v>
@@ -11529,7 +11529,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:23" s="68" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" s="55" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="46">
         <v>455</v>
       </c>
@@ -11546,7 +11546,7 @@
         <v>380</v>
       </c>
       <c r="F172" s="53" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="G172" s="49" t="s">
         <v>575</v>
@@ -18663,15 +18663,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18933,27 +18930,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18978,9 +18969,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
ID 35, 43, essendo stata dichiarata la non applicabilità, è sufficiente compilare il campo "razionale di applicabilità"; vi chiediamo pertanto di non valorizzare le colonne da M a S;
ID 51, il caso di time-out è sempre applicabile, per cui è necessario rivedere la compilazione della colonna “J” e valorizzare le colonne relative alla gestione dell’errore (da “P” a “S”).
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IG.PSO/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IG.PSO/IGSUITE/4.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IG.PSO\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF17550-9EB1-43F2-8520-C8CA062BC57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FAE569-0155-48F8-862B-213806F4F2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="579">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2434,6 +2434,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120212.4.4.a35bbca880792ec85936360b5b135c449fc79cfd848419b4ac36b75890a6a81b.d51b7f90a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Error calling Validate: Host sconosciuto. (modipa-val.fse.salute.gov.it:443)</t>
   </si>
 </sst>
 </file>
@@ -4547,10 +4550,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F172" sqref="F172"/>
+      <selection pane="bottomRight" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5160,25 +5163,13 @@
         <v>232</v>
       </c>
       <c r="L18" s="45"/>
-      <c r="M18" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="N18" s="45" t="s">
-        <v>228</v>
-      </c>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
       <c r="O18" s="45"/>
-      <c r="P18" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q18" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="R18" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="S18" s="45" t="s">
-        <v>449</v>
-      </c>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
       <c r="T18" s="45" t="s">
         <v>226</v>
       </c>
@@ -5476,25 +5467,13 @@
         <v>232</v>
       </c>
       <c r="L26" s="45"/>
-      <c r="M26" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26" s="45" t="s">
-        <v>228</v>
-      </c>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
       <c r="O26" s="45"/>
-      <c r="P26" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q26" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="R26" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="S26" s="45" t="s">
-        <v>449</v>
-      </c>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
       <c r="T26" s="45" t="s">
         <v>226</v>
       </c>
@@ -5800,7 +5779,7 @@
       <c r="H34" s="49"/>
       <c r="I34" s="50"/>
       <c r="J34" s="45" t="s">
-        <v>228</v>
+        <v>64</v>
       </c>
       <c r="K34" s="45" t="s">
         <v>237</v>
@@ -5814,7 +5793,9 @@
       <c r="N34" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="O34" s="45"/>
+      <c r="O34" s="45" t="s">
+        <v>578</v>
+      </c>
       <c r="P34" s="45" t="s">
         <v>64</v>
       </c>

</xml_diff>